<commit_message>
Add 15 Product templates with correct industry content
</commit_message>
<xml_diff>
--- a/static/templates/Product_Change_Management_Plan.xlsx
+++ b/static/templates/Product_Change_Management_Plan.xlsx
@@ -557,7 +557,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>PRODUCT Change Management Plan Project</t>
+          <t>Product Development Implementation Project</t>
         </is>
       </c>
     </row>
@@ -584,7 +584,7 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>Enterprise AI/ML Implementation</t>
+          <t>Enterprise Product Development Implementation</t>
         </is>
       </c>
     </row>
@@ -660,6 +660,7 @@
         </is>
       </c>
     </row>
+    <row r="13"/>
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
@@ -670,7 +671,7 @@
     <row r="15">
       <c r="A15" s="5" t="inlineStr">
         <is>
-          <t>1. Achieve 95% user adoption of new AI/ML systems within 6 months of go-live</t>
+          <t>1. Achieve 95% user adoption of new Product Development systems within 6 months of go-live</t>
         </is>
       </c>
       <c r="B15" s="6" t="n"/>
@@ -698,7 +699,7 @@
     <row r="17">
       <c r="A17" s="5" t="inlineStr">
         <is>
-          <t>3. Build organizational capability and confidence in AI/ML technologies</t>
+          <t>3. Build organizational capability and confidence in Product Development technologies</t>
         </is>
       </c>
       <c r="B17" s="6" t="n"/>
@@ -740,7 +741,7 @@
     <row r="20">
       <c r="A20" s="5" t="inlineStr">
         <is>
-          <t>6. Create positive stakeholder sentiment and enthusiasm for AI/ML transformation</t>
+          <t>6. Create positive stakeholder sentiment and enthusiasm for Product Development transformation</t>
         </is>
       </c>
       <c r="B20" s="6" t="n"/>
@@ -751,6 +752,7 @@
       <c r="G20" s="6" t="n"/>
       <c r="H20" s="7" t="n"/>
     </row>
+    <row r="21"/>
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
@@ -902,6 +904,7 @@
         </is>
       </c>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" s="9" t="inlineStr">
         <is>
@@ -995,7 +998,7 @@
       </c>
       <c r="G4" s="5" t="inlineStr">
         <is>
-          <t>AI/ML automation</t>
+          <t>Product Development automation</t>
         </is>
       </c>
       <c r="H4" s="5" t="inlineStr">
@@ -1055,7 +1058,7 @@
       </c>
       <c r="G5" s="5" t="inlineStr">
         <is>
-          <t>AI-powered insights</t>
+          <t>Product-powered insights</t>
         </is>
       </c>
       <c r="H5" s="5" t="inlineStr">
@@ -1175,7 +1178,7 @@
       </c>
       <c r="G7" s="5" t="inlineStr">
         <is>
-          <t>New AI interface</t>
+          <t>New Product interface</t>
         </is>
       </c>
       <c r="H7" s="5" t="inlineStr">
@@ -1415,7 +1418,7 @@
       </c>
       <c r="G11" s="5" t="inlineStr">
         <is>
-          <t>AI-enhanced CRM</t>
+          <t>Product-enhanced CRM</t>
         </is>
       </c>
       <c r="H11" s="5" t="inlineStr">
@@ -1475,7 +1478,7 @@
       </c>
       <c r="G12" s="5" t="inlineStr">
         <is>
-          <t>AI-assisted support</t>
+          <t>Product-assisted support</t>
         </is>
       </c>
       <c r="H12" s="5" t="inlineStr">
@@ -1535,7 +1538,7 @@
       </c>
       <c r="G13" s="5" t="inlineStr">
         <is>
-          <t>AI-powered testing</t>
+          <t>Product-powered testing</t>
         </is>
       </c>
       <c r="H13" s="5" t="inlineStr">
@@ -1737,6 +1740,7 @@
         </is>
       </c>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" s="9" t="inlineStr">
         <is>

</xml_diff>